<commit_message>
refatoracao e add excelConsumer
</commit_message>
<xml_diff>
--- a/src/test/resources/dataBase/BDD_AdvantageOnlineShoppingData.xlsx
+++ b/src/test/resources/dataBase/BDD_AdvantageOnlineShoppingData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george.junior\eclipse-XPTO\TDD_AdvantageOnlineShopping\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george.junior\eclipse-XPTO\BDD_AdvantageOnlineShopping\src\test\resources\dataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04FFF27-3FD6-4556-BEF7-9DD8BF1F0C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2C8A2C-7D6A-4482-80D6-1AE0AFAD520A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="2070" windowWidth="20730" windowHeight="11160" tabRatio="586" firstSheet="3" activeTab="3" xr2:uid="{D4DEB64E-DE7E-45FC-8D49-61962D919F60}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="586" firstSheet="3" activeTab="3" xr2:uid="{D4DEB64E-DE7E-45FC-8D49-61962D919F60}"/>
   </bookViews>
   <sheets>
     <sheet name="AcessarUmProdutoPelaHome_Po" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="50">
   <si>
     <t>produto</t>
   </si>
@@ -183,6 +185,9 @@
   </si>
   <si>
     <t>DeveTentarCadasTrarUmNovoClienteComFalha</t>
+  </si>
+  <si>
+    <t>teste.com</t>
   </si>
 </sst>
 </file>
@@ -880,7 +885,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,7 +951,7 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>21</v>
@@ -1022,7 +1027,7 @@
         <v>31</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
         <v>22</v>
@@ -1053,7 +1058,7 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{2F4CF434-4928-472C-A45E-A687B9060E04}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{24419471-4843-4B96-B5A2-9D74ABF59607}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{078ED41D-26D8-43FD-B40F-97DEB41719AB}"/>
+    <hyperlink ref="E4" r:id="rId3" display="teste1@teste.com" xr:uid="{078ED41D-26D8-43FD-B40F-97DEB41719AB}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>